<commit_message>
add modules + fix bugs
</commit_message>
<xml_diff>
--- a/rxn_bounds/R3D301_EX_rxns.xlsx
+++ b/rxn_bounds/R3D301_EX_rxns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prins\GitHub\Human1_RPE-PR\rxn_bounds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E032C1-CA2B-4DB5-9D1B-B8ABDA96A0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DDF25D-8539-445C-AD5F-8BBFBB48C2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{69497B25-CBDB-B04B-AD57-06C30CF64D2B}"/>
+    <workbookView minimized="1" xWindow="3252" yWindow="3000" windowWidth="19116" windowHeight="9960" xr2:uid="{69497B25-CBDB-B04B-AD57-06C30CF64D2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -11971,9 +11971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE23A8E-EE2C-E84B-B990-91F05B962947}">
   <dimension ref="A1:E1638"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>